<commit_message>
renamed pubic symphysis columns for clarity
</commit_message>
<xml_diff>
--- a/SettlementDimorphismRawData.xlsx
+++ b/SettlementDimorphismRawData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfeil\Documents\Professional\Ongoing Research\Settlement and SD\dutch.settlement.dimorphism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6563D337-815E-4B1E-ACF5-5C7ADE66BCBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1778F4E-03EE-4A4F-BB0A-FE3107BE2DB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{C318A678-435F-464B-BB32-1C41A62A3D21}"/>
   </bookViews>
@@ -113,12 +113,6 @@
     <t>R Apical</t>
   </si>
   <si>
-    <t>L Pubic</t>
-  </si>
-  <si>
-    <t>R Pubic</t>
-  </si>
-  <si>
     <t>S360V0762</t>
   </si>
   <si>
@@ -714,6 +708,12 @@
   </si>
   <si>
     <t>OA</t>
+  </si>
+  <si>
+    <t>L Pubic Symphysis</t>
+  </si>
+  <si>
+    <t>R Pubic Symphysis</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E93568-27E6-43A3-97A0-78C98F4AAEA7}">
   <dimension ref="A1:AG200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1129,13 +1129,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -1213,27 +1213,27 @@
         <v>25</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>26</v>
+        <v>225</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>27</v>
+        <v>226</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E2" s="5">
         <v>4</v>
@@ -1316,16 +1316,16 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E3" s="5">
         <v>3</v>
@@ -1400,16 +1400,16 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -1490,16 +1490,16 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E5" s="5">
         <v>3</v>
@@ -1566,16 +1566,16 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E6" s="5">
         <v>4</v>
@@ -1662,16 +1662,16 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="E7" s="5">
         <v>2</v>
@@ -1756,16 +1756,16 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E8" s="5">
         <v>5</v>
@@ -1852,16 +1852,16 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E9" s="5">
         <v>5</v>
@@ -1948,16 +1948,16 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -2044,16 +2044,16 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E11" s="5">
         <v>2</v>
@@ -2138,16 +2138,16 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E12" s="5">
         <v>4</v>
@@ -2234,16 +2234,16 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E13" s="5">
         <v>4</v>
@@ -2324,16 +2324,16 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E14" s="5">
         <v>5</v>
@@ -2398,16 +2398,16 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E15" s="5">
         <v>3</v>
@@ -2492,16 +2492,16 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E16" s="5">
         <v>2</v>
@@ -2572,16 +2572,16 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E17" s="5">
         <v>3</v>
@@ -2666,16 +2666,16 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="E18" s="5">
         <v>3</v>
@@ -2746,16 +2746,16 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E19" s="5">
         <v>4</v>
@@ -2822,16 +2822,16 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E20" s="5">
         <v>3</v>
@@ -2918,16 +2918,16 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E21" s="5">
         <v>4</v>
@@ -2984,16 +2984,16 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -3058,16 +3058,16 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E23" s="5">
         <v>4</v>
@@ -3154,16 +3154,16 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E24" s="5">
         <v>3</v>
@@ -3224,16 +3224,16 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E25" s="5">
         <v>3</v>
@@ -3304,16 +3304,16 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5">
@@ -3396,16 +3396,16 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E27" s="5">
         <v>2</v>
@@ -3492,16 +3492,16 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
@@ -3588,16 +3588,16 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E29" s="5">
         <v>4</v>
@@ -3674,16 +3674,16 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E30" s="5">
         <v>3</v>
@@ -3770,16 +3770,16 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E31" s="5">
         <v>2</v>
@@ -3862,16 +3862,16 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E32" s="5">
         <v>3</v>
@@ -3958,16 +3958,16 @@
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E33" s="5">
         <v>5</v>
@@ -4046,16 +4046,16 @@
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E34" s="5">
         <v>2</v>
@@ -4134,16 +4134,16 @@
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5">
@@ -4210,16 +4210,16 @@
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E36" s="5">
         <v>4</v>
@@ -4306,16 +4306,16 @@
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="E37" s="5">
         <v>2</v>
@@ -4402,16 +4402,16 @@
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E38" s="5">
         <v>4</v>
@@ -4490,16 +4490,16 @@
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E39" s="5">
         <v>2</v>
@@ -4584,16 +4584,16 @@
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E40" s="5">
         <v>4</v>
@@ -4662,16 +4662,16 @@
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E41" s="5">
         <v>2</v>
@@ -4748,16 +4748,16 @@
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A42" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E42" s="5">
         <v>1</v>
@@ -4836,16 +4836,16 @@
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A43" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E43" s="5">
         <v>2</v>
@@ -4922,16 +4922,16 @@
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C44" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E44" s="5">
         <v>5</v>
@@ -5018,16 +5018,16 @@
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A45" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5">
@@ -5112,16 +5112,16 @@
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A46" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5">
@@ -5206,16 +5206,16 @@
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C47" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E47" s="5">
         <v>4</v>
@@ -5302,16 +5302,16 @@
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E48" s="5">
         <v>5</v>
@@ -5398,16 +5398,16 @@
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C49" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E49" s="5">
         <v>5</v>
@@ -5486,16 +5486,16 @@
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E50" s="5">
         <v>4</v>
@@ -5582,16 +5582,16 @@
     </row>
     <row r="51" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E51" s="5">
         <v>5</v>
@@ -5656,16 +5656,16 @@
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A52" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C52" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E52" s="5">
         <v>1</v>
@@ -5748,16 +5748,16 @@
     </row>
     <row r="53" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A53" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C53" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E53" s="5">
         <v>5</v>
@@ -5838,16 +5838,16 @@
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A54" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C54" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E54" s="5">
         <v>4</v>
@@ -5934,16 +5934,16 @@
     </row>
     <row r="55" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A55" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E55" s="5">
         <v>4</v>
@@ -6030,16 +6030,16 @@
     </row>
     <row r="56" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A56" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C56" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E56" s="5">
         <v>5</v>
@@ -6110,16 +6110,16 @@
     </row>
     <row r="57" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A57" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E57" s="5">
         <v>3</v>
@@ -6206,16 +6206,16 @@
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A58" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E58" s="5">
         <v>4</v>
@@ -6302,16 +6302,16 @@
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A59" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E59" s="5">
         <v>4</v>
@@ -6386,16 +6386,16 @@
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A60" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E60" s="5">
         <v>5</v>
@@ -6470,16 +6470,16 @@
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A61" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C61" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E61" s="5">
         <v>4</v>
@@ -6560,16 +6560,16 @@
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A62" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C62" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E62" s="5">
         <v>4</v>
@@ -6646,16 +6646,16 @@
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A63" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C63" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E63" s="5">
         <v>5</v>
@@ -6734,16 +6734,16 @@
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A64" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E64" s="5">
         <v>5</v>
@@ -6828,16 +6828,16 @@
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A65" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C65" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5">
@@ -6912,16 +6912,16 @@
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A66" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E66" s="5">
         <v>5</v>
@@ -6990,16 +6990,16 @@
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A67" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E67" s="5">
         <v>4</v>
@@ -7058,16 +7058,16 @@
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A68" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C68" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E68" s="5">
         <v>5</v>
@@ -7126,16 +7126,16 @@
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A69" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E69" s="5">
         <v>2</v>
@@ -7206,16 +7206,16 @@
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A70" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E70" s="5">
         <v>1</v>
@@ -7292,16 +7292,16 @@
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A71" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C71" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E71" s="5">
         <v>4</v>
@@ -7388,16 +7388,16 @@
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A72" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C72" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E72" s="5">
         <v>5</v>
@@ -7468,16 +7468,16 @@
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A73" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C73" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E73" s="5">
         <v>1</v>
@@ -7564,16 +7564,16 @@
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A74" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E74" s="5">
         <v>5</v>
@@ -7638,16 +7638,16 @@
     </row>
     <row r="75" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A75" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E75" s="5">
         <v>3</v>
@@ -7734,16 +7734,16 @@
     </row>
     <row r="76" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A76" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C76" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E76" s="5">
         <v>5</v>
@@ -7824,16 +7824,16 @@
     </row>
     <row r="77" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A77" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E77" s="5">
         <v>4</v>
@@ -7920,16 +7920,16 @@
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A78" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C78" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E78" s="5">
         <v>3</v>
@@ -7998,16 +7998,16 @@
     </row>
     <row r="79" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A79" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C79" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E79" s="5">
         <v>4</v>
@@ -8094,16 +8094,16 @@
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A80" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E80" s="5">
         <v>2</v>
@@ -8174,16 +8174,16 @@
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A81" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C81" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D81" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E81" s="5">
         <v>4</v>
@@ -8266,16 +8266,16 @@
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A82" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E82" s="5">
         <v>4</v>
@@ -8362,16 +8362,16 @@
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A83" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E83" s="5">
         <v>5</v>
@@ -8438,16 +8438,16 @@
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A84" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C84" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D84" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E84" s="5">
         <v>4</v>
@@ -8532,16 +8532,16 @@
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A85" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C85" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D85" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E85" s="5">
         <v>5</v>
@@ -8620,16 +8620,16 @@
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A86" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C86" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D86" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E86" s="5"/>
       <c r="F86" s="5">
@@ -8714,16 +8714,16 @@
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A87" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E87" s="5">
         <v>5</v>
@@ -8802,16 +8802,16 @@
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A88" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C88" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E88" s="5">
         <v>5</v>
@@ -8898,16 +8898,16 @@
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A89" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C89" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E89" s="5">
         <v>1</v>
@@ -8994,16 +8994,16 @@
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A90" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C90" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E90" s="5">
         <v>4</v>
@@ -9068,16 +9068,16 @@
     </row>
     <row r="91" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A91" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C91" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E91" s="5">
         <v>2</v>
@@ -9164,16 +9164,16 @@
     </row>
     <row r="92" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A92" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E92" s="5">
         <v>4</v>
@@ -9258,16 +9258,16 @@
     </row>
     <row r="93" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A93" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C93" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D93" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="E93" s="7">
         <v>3</v>
@@ -9353,16 +9353,16 @@
     </row>
     <row r="94" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A94" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C94" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D94" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="E94" s="7"/>
       <c r="F94" s="7">
@@ -9438,16 +9438,16 @@
     </row>
     <row r="95" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A95" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C95" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D95" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="E95" s="7">
         <v>1</v>
@@ -9523,16 +9523,16 @@
     </row>
     <row r="96" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A96" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E96" s="7">
         <v>1</v>
@@ -9604,16 +9604,16 @@
     </row>
     <row r="97" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A97" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E97" s="7">
         <v>1</v>
@@ -9699,16 +9699,16 @@
     </row>
     <row r="98" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A98" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
@@ -9790,16 +9790,16 @@
     </row>
     <row r="99" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A99" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E99" s="7">
         <v>2</v>
@@ -9887,16 +9887,16 @@
     </row>
     <row r="100" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A100" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E100" s="7">
         <v>2</v>
@@ -9964,16 +9964,16 @@
     </row>
     <row r="101" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A101" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E101" s="7">
         <v>2</v>
@@ -10063,16 +10063,16 @@
     </row>
     <row r="102" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A102" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E102" s="7">
         <v>2</v>
@@ -10160,16 +10160,16 @@
     </row>
     <row r="103" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A103" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E103" s="7">
         <v>2</v>
@@ -10249,16 +10249,16 @@
     </row>
     <row r="104" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A104" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E104" s="7">
         <v>5</v>
@@ -10346,16 +10346,16 @@
     </row>
     <row r="105" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A105" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E105" s="7">
         <v>1</v>
@@ -10431,16 +10431,16 @@
     </row>
     <row r="106" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A106" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E106" s="7">
         <v>3</v>
@@ -10528,16 +10528,16 @@
     </row>
     <row r="107" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A107" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E107" s="7">
         <v>5</v>
@@ -10613,16 +10613,16 @@
     </row>
     <row r="108" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A108" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E108" s="7">
         <v>2</v>
@@ -10698,16 +10698,16 @@
     </row>
     <row r="109" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A109" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E109" s="7">
         <v>1</v>
@@ -10779,16 +10779,16 @@
     </row>
     <row r="110" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A110" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E110" s="7">
         <v>1</v>
@@ -10862,16 +10862,16 @@
     </row>
     <row r="111" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A111" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E111" s="7">
         <v>1</v>
@@ -10959,16 +10959,16 @@
     </row>
     <row r="112" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A112" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E112" s="7">
         <v>3</v>
@@ -11048,16 +11048,16 @@
     </row>
     <row r="113" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A113" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E113" s="7">
         <v>1</v>
@@ -11127,16 +11127,16 @@
     </row>
     <row r="114" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A114" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E114" s="7">
         <v>4</v>
@@ -11224,16 +11224,16 @@
     </row>
     <row r="115" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A115" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E115" s="7">
         <v>4</v>
@@ -11319,16 +11319,16 @@
     </row>
     <row r="116" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A116" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E116" s="7">
         <v>3</v>
@@ -11402,16 +11402,16 @@
     </row>
     <row r="117" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A117" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E117" s="7">
         <v>5</v>
@@ -11501,16 +11501,16 @@
     </row>
     <row r="118" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A118" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E118" s="7">
         <v>1</v>
@@ -11586,16 +11586,16 @@
     </row>
     <row r="119" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A119" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E119" s="7">
         <v>4</v>
@@ -11665,16 +11665,16 @@
     </row>
     <row r="120" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A120" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E120" s="7">
         <v>3</v>
@@ -11742,16 +11742,16 @@
     </row>
     <row r="121" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A121" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E121" s="7">
         <v>1</v>
@@ -11823,16 +11823,16 @@
     </row>
     <row r="122" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A122" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E122" s="7">
         <v>4</v>
@@ -11910,16 +11910,16 @@
     </row>
     <row r="123" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A123" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E123" s="7">
         <v>1</v>
@@ -11991,16 +11991,16 @@
     </row>
     <row r="124" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A124" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E124" s="7">
         <v>2</v>
@@ -12072,16 +12072,16 @@
     </row>
     <row r="125" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A125" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E125" s="7">
         <v>4</v>
@@ -12167,16 +12167,16 @@
     </row>
     <row r="126" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A126" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E126" s="7">
         <v>1</v>
@@ -12242,16 +12242,16 @@
     </row>
     <row r="127" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A127" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E127" s="7">
         <v>2</v>
@@ -12339,16 +12339,16 @@
     </row>
     <row r="128" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A128" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E128" s="7">
         <v>1</v>
@@ -12432,16 +12432,16 @@
     </row>
     <row r="129" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A129" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E129" s="7">
         <v>1</v>
@@ -12513,16 +12513,16 @@
     </row>
     <row r="130" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A130" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E130" s="7">
         <v>1</v>
@@ -12608,16 +12608,16 @@
     </row>
     <row r="131" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A131" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E131" s="7">
         <v>1</v>
@@ -12689,16 +12689,16 @@
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A132" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E132" s="7">
         <v>4</v>
@@ -12786,16 +12786,16 @@
     </row>
     <row r="133" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A133" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E133" s="7">
         <v>5</v>
@@ -12867,16 +12867,16 @@
     </row>
     <row r="134" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A134" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E134" s="7">
         <v>1</v>
@@ -12944,16 +12944,16 @@
     </row>
     <row r="135" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A135" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E135" s="7">
         <v>2</v>
@@ -13031,16 +13031,16 @@
     </row>
     <row r="136" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A136" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E136" s="7">
         <v>1</v>
@@ -13124,16 +13124,16 @@
     </row>
     <row r="137" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A137" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" s="7"/>
@@ -13199,16 +13199,16 @@
     </row>
     <row r="138" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A138" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E138" s="7">
         <v>5</v>
@@ -13280,16 +13280,16 @@
     </row>
     <row r="139" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A139" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E139" s="7">
         <v>2</v>
@@ -13367,16 +13367,16 @@
     </row>
     <row r="140" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A140" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E140" s="7">
         <v>1</v>
@@ -13464,16 +13464,16 @@
     </row>
     <row r="141" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A141" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E141" s="7">
         <v>4</v>
@@ -13535,16 +13535,16 @@
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A142" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E142" s="7">
         <v>4</v>
@@ -13616,16 +13616,16 @@
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A143" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E143" s="7">
         <v>5</v>
@@ -13711,16 +13711,16 @@
     </row>
     <row r="144" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A144" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E144" s="7">
         <v>3</v>
@@ -13808,16 +13808,16 @@
     </row>
     <row r="145" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A145" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E145" s="7">
         <v>3</v>
@@ -13883,16 +13883,16 @@
     </row>
     <row r="146" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A146" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C146" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D146" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D146" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E146" s="7">
         <v>3</v>
@@ -13970,16 +13970,16 @@
     </row>
     <row r="147" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A147" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C147" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D147" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D147" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E147" s="7">
         <v>4</v>
@@ -14067,16 +14067,16 @@
     </row>
     <row r="148" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A148" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C148" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D148" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D148" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E148" s="7">
         <v>5</v>
@@ -14164,16 +14164,16 @@
     </row>
     <row r="149" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A149" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C149" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D149" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D149" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E149" s="7">
         <v>5</v>
@@ -14261,16 +14261,16 @@
     </row>
     <row r="150" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A150" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C150" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D150" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D150" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E150" s="7">
         <v>5</v>
@@ -14342,16 +14342,16 @@
     </row>
     <row r="151" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A151" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C151" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D151" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D151" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E151" s="7">
         <v>4</v>
@@ -14415,16 +14415,16 @@
     </row>
     <row r="152" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A152" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C152" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D152" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D152" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E152" s="7">
         <v>4</v>
@@ -14512,16 +14512,16 @@
     </row>
     <row r="153" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A153" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C153" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D153" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D153" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E153" s="7">
         <v>1</v>
@@ -14597,16 +14597,16 @@
     </row>
     <row r="154" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A154" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C154" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D154" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D154" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E154" s="7">
         <v>5</v>
@@ -14680,16 +14680,16 @@
     </row>
     <row r="155" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A155" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C155" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D155" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D155" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E155" s="7">
         <v>5</v>
@@ -14759,16 +14759,16 @@
     </row>
     <row r="156" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A156" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C156" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D156" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D156" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E156" s="7">
         <v>2</v>
@@ -14848,16 +14848,16 @@
     </row>
     <row r="157" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A157" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C157" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D157" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D157" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E157" s="7">
         <v>5</v>
@@ -14927,16 +14927,16 @@
     </row>
     <row r="158" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A158" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C158" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D158" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D158" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E158" s="7">
         <v>2</v>
@@ -15024,16 +15024,16 @@
     </row>
     <row r="159" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A159" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C159" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D159" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D159" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E159" s="7">
         <v>4</v>
@@ -15113,16 +15113,16 @@
     </row>
     <row r="160" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A160" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C160" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D160" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D160" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E160" s="7">
         <v>3</v>
@@ -15192,16 +15192,16 @@
     </row>
     <row r="161" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A161" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C161" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D161" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D161" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E161" s="7">
         <v>5</v>
@@ -15289,16 +15289,16 @@
     </row>
     <row r="162" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A162" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C162" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D162" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D162" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E162" s="7">
         <v>3</v>
@@ -15370,16 +15370,16 @@
     </row>
     <row r="163" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A163" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E163" s="7">
         <v>3</v>
@@ -15457,16 +15457,16 @@
     </row>
     <row r="164" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A164" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E164" s="7">
         <v>4</v>
@@ -15554,16 +15554,16 @@
     </row>
     <row r="165" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A165" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E165" s="7">
         <v>2</v>
@@ -15649,16 +15649,16 @@
     </row>
     <row r="166" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A166" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E166" s="7">
         <v>2</v>
@@ -15746,16 +15746,16 @@
     </row>
     <row r="167" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A167" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E167" s="7">
         <v>5</v>
@@ -15829,16 +15829,16 @@
     </row>
     <row r="168" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A168" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E168" s="7">
         <v>5</v>
@@ -15926,16 +15926,16 @@
     </row>
     <row r="169" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A169" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E169" s="7">
         <v>2</v>
@@ -16013,16 +16013,16 @@
     </row>
     <row r="170" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A170" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E170" s="7">
         <v>5</v>
@@ -16112,16 +16112,16 @@
     </row>
     <row r="171" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A171" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E171" s="7">
         <v>5</v>
@@ -16205,16 +16205,16 @@
     </row>
     <row r="172" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A172" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E172" s="7">
         <v>5</v>
@@ -16282,16 +16282,16 @@
     </row>
     <row r="173" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A173" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E173" s="7">
         <v>4</v>
@@ -16377,16 +16377,16 @@
     </row>
     <row r="174" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A174" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D174" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E174" s="7"/>
       <c r="F174" s="7">
@@ -16468,16 +16468,16 @@
     </row>
     <row r="175" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A175" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E175" s="7">
         <v>4</v>
@@ -16561,16 +16561,16 @@
     </row>
     <row r="176" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A176" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E176" s="7">
         <v>5</v>
@@ -16642,16 +16642,16 @@
     </row>
     <row r="177" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A177" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E177" s="7">
         <v>3</v>
@@ -16739,16 +16739,16 @@
     </row>
     <row r="178" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A178" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E178" s="7">
         <v>4</v>
@@ -16836,16 +16836,16 @@
     </row>
     <row r="179" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A179" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D179" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E179" s="7">
         <v>5</v>
@@ -16917,16 +16917,16 @@
     </row>
     <row r="180" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A180" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D180" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E180" s="7">
         <v>5</v>
@@ -17010,16 +17010,16 @@
     </row>
     <row r="181" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A181" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E181" s="7">
         <v>5</v>
@@ -17103,16 +17103,16 @@
     </row>
     <row r="182" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A182" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D182" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E182" s="7"/>
       <c r="F182" s="7">
@@ -17192,16 +17192,16 @@
     </row>
     <row r="183" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A183" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E183" s="7">
         <v>4</v>
@@ -17283,16 +17283,16 @@
     </row>
     <row r="184" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A184" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E184" s="7">
         <v>4</v>
@@ -17364,16 +17364,16 @@
     </row>
     <row r="185" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A185" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E185" s="7">
         <v>4</v>
@@ -17457,16 +17457,16 @@
     </row>
     <row r="186" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A186" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E186" s="7">
         <v>5</v>
@@ -17554,16 +17554,16 @@
     </row>
     <row r="187" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A187" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E187" s="7">
         <v>5</v>
@@ -17647,16 +17647,16 @@
     </row>
     <row r="188" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A188" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E188" s="7">
         <v>2</v>

</xml_diff>